<commit_message>
(Issue #23) Finalized MoverUnpacker eFSM design in excel file.  No updates to graphic.
</commit_message>
<xml_diff>
--- a/docs/MoverUnpackerDesign.xlsx
+++ b/docs/MoverUnpackerDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Projects/OrchestrationRuntime/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0377BDC3-692C-9D4B-B94F-5C91052EA704}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50E3ECF-A488-DD47-B283-00E2F2E5ADF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="440" windowWidth="42380" windowHeight="27600" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
+    <workbookView xWindow="24100" yWindow="440" windowWidth="27100" windowHeight="27600" xr2:uid="{9B8D0C4A-3FF1-A04E-B8F8-B86CE3BC2D78}"/>
   </bookViews>
   <sheets>
     <sheet name="Design_1.0" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="40">
   <si>
     <t>Machine Mode</t>
   </si>
@@ -42,45 +42,13 @@
     <t>Running_Open</t>
   </si>
   <si>
-    <t>Event Input</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>increaseThreadCount(i)</t>
-  </si>
-  <si>
     <t>Nothing</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Throw error </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- cannot close a queue if machine isn't running</t>
-    </r>
-  </si>
-  <si>
     <t>any</t>
-  </si>
-  <si>
-    <t>any i</t>
   </si>
   <si>
     <t>Current State</t>
@@ -191,35 +159,6 @@
     <t>N_T &gt; 0</t>
   </si>
   <si>
-    <t>startTask</t>
-  </si>
-  <si>
-    <t>startCycle</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Throw error</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Cannot be thread receiver</t>
-    </r>
-  </si>
-  <si>
     <t>closeQueue()</t>
   </si>
   <si>
@@ -227,9 +166,6 @@
   </si>
   <si>
     <t>N_T+1 &gt; 0</t>
-  </si>
-  <si>
-    <t>Initiate asynchronous transfer &amp; register callback for post-transfer handling</t>
   </si>
   <si>
     <r>
@@ -259,9 +195,6 @@
     <t>N_T-1 &gt;= 0</t>
   </si>
   <si>
-    <t>any I</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -286,9 +219,6 @@
   </si>
   <si>
     <t>enqueue(D)</t>
-  </si>
-  <si>
-    <t>any D</t>
   </si>
   <si>
     <t>N_T &gt; 1</t>
@@ -330,6 +260,55 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">Throw error </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- adding data item in Idle is prohibited</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IMPOSSIBLE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This event can only occur if N_T &gt; 0</t>
+    </r>
+  </si>
+  <si>
+    <t>N_T &gt;= 0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>IMPOSSIBLE</t>
     </r>
     <r>
@@ -340,7 +319,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: Starts in Idle with 0 and all transitions to Idle have 0.  No valid event for Idle increases N_T.</t>
+      <t>: Starts in Idle with 0 and all transitions to Idle have 0.  No event in Idle increases N_T.</t>
     </r>
   </si>
   <si>
@@ -363,7 +342,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- adding data item in Idle is prohibited</t>
+      <t>- cannot close a queue if it isn't already open</t>
     </r>
   </si>
   <si>
@@ -376,6 +355,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">Throw error </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- cannot start cycle until this cycle finishes</t>
+    </r>
+  </si>
+  <si>
+    <t>startCycle()</t>
+  </si>
+  <si>
+    <t>Initiate asynchronous D-to-H transfer &amp; register callback for post-transfer handling</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>IMPOSSIBLE:</t>
     </r>
     <r>
@@ -386,33 +394,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> This event can only occur if N_T &gt; 0</t>
-    </r>
-  </si>
-  <si>
-    <t>N_T &gt;= 0</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IMPOSSIBLE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Transitions to Closed only if N_T &gt; 0.  Transition from Closed to Idle if </t>
+      <t xml:space="preserve"> Transitions to Closed only if N_T &gt; 0.  </t>
     </r>
     <r>
       <rPr>
@@ -431,7 +413,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> occurs with N_T = 1</t>
+      <t xml:space="preserve"> is only event that can decrease N_T and it causes transition from Closed to Idle if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>transferFinished</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> occurs with N_T = 1. </t>
     </r>
   </si>
 </sst>
@@ -526,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -581,19 +582,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -629,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,10 +631,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -706,7 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -727,7 +712,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1050,11 +1035,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L35"/>
+  <dimension ref="B1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1065,681 +1050,542 @@
     <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="66.83203125" style="16" customWidth="1"/>
-    <col min="11" max="11" width="31.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="99.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="83.6640625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="31.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="99.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="72.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="16" customHeight="1">
-      <c r="B1" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-    </row>
-    <row r="2" spans="2:12" ht="17" thickBot="1">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-    </row>
-    <row r="3" spans="2:12" ht="17" thickBot="1">
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="33"/>
-      <c r="H3" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="2:12" ht="17" thickBot="1">
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+    <row r="1" spans="2:11" ht="16" customHeight="1">
+      <c r="B1" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+    </row>
+    <row r="2" spans="2:11" ht="17" thickBot="1">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+    </row>
+    <row r="3" spans="2:11" ht="17" thickBot="1">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="G3" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" spans="2:11" ht="17" thickBot="1">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="26"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="26"/>
-    </row>
-    <row r="5" spans="2:12" ht="18" thickBot="1">
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="E4" s="25"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" spans="2:11" ht="18" thickBot="1">
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>22</v>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="17" t="s">
+      <c r="H5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="2:12" ht="17">
-      <c r="B6" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="13" t="s">
+      <c r="J5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="2:11" ht="17">
+      <c r="B6" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="2:12" ht="34">
-      <c r="B7" s="22"/>
-      <c r="C7" s="24"/>
+        <v>5</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="2:11" ht="17" customHeight="1">
+      <c r="B7" s="21"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="2:12" ht="17">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+        <v>5</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="2:11" ht="17">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>25</v>
+      <c r="F8" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:12" ht="17">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="2:11" ht="17">
+      <c r="B9" s="21"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>7</v>
+      <c r="F9" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="2:12" ht="17">
-      <c r="B10" s="22"/>
-      <c r="C10" s="25"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="2:11" ht="17">
+      <c r="B10" s="21"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="2:12" ht="17">
-      <c r="B11" s="22"/>
-      <c r="C11" s="25"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="2:11" ht="17">
+      <c r="B11" s="21"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>27</v>
+      <c r="F11" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="2:12" ht="17">
-      <c r="B12" s="22"/>
-      <c r="C12" s="25"/>
+        <v>5</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="26"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="2:11" ht="17">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="27"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="2:12" ht="17">
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+        <v>4</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="2:11" ht="18" customHeight="1">
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="2:12" ht="17">
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
+        <v>22</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="2:11" ht="17">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>7</v>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="2:12" ht="18" customHeight="1">
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="2:12" ht="17">
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+        <v>3</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="2:11" ht="17" customHeight="1">
+      <c r="C15" s="11"/>
+      <c r="F15" s="10"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="26"/>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" spans="2:11" ht="17">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="27"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="2:11" ht="17">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="3">
+      <c r="F17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
         <v>0</v>
       </c>
-      <c r="J16" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="2:12" ht="17" customHeight="1">
-      <c r="C17" s="12"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="27"/>
-      <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="2:12" ht="17">
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
+      <c r="I17" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="28"/>
+    </row>
+    <row r="18" spans="2:11" ht="17">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="2:12" ht="17">
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
+        <v>19</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" ht="34">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
       <c r="F19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="2:11" ht="17">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="2:11" ht="17">
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="2:11" ht="17">
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="2:11" ht="17">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="2:11" ht="17">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="K19" s="29"/>
-    </row>
-    <row r="20" spans="2:12" ht="17">
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="I24" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" ht="17" customHeight="1">
+      <c r="C25" s="11"/>
+      <c r="F25" s="9"/>
+      <c r="I25" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="2:12" ht="34">
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="14"/>
-    </row>
-    <row r="22" spans="2:12" ht="17">
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J22" s="16" t="s">
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="2:11" ht="17" customHeight="1">
+      <c r="F26" s="9"/>
+      <c r="I26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="2:12" ht="17">
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="2:12" ht="17">
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="2:12" ht="17">
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="2:12" ht="17">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="K26" s="10"/>
-    </row>
-    <row r="27" spans="2:12" ht="17">
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="2:12" ht="17" customHeight="1">
-      <c r="C28" s="12"/>
-      <c r="F28" s="10"/>
-      <c r="J28" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="2:12" ht="17" customHeight="1">
-      <c r="F29" s="10"/>
-      <c r="J29" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="2:12">
-      <c r="F30" s="10"/>
-      <c r="J30" s="20"/>
-      <c r="L30"/>
-    </row>
-    <row r="31" spans="2:12">
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="2:12">
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="F27" s="9"/>
+      <c r="I27" s="19"/>
+      <c r="K27"/>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="2:11">
       <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="6:6">
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="6:6">
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="6:6">
-      <c r="F35" s="10"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0"/>
@@ -1748,8 +1594,8 @@
     <mergeCell ref="C1:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="30" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>